<commit_message>
PoN: finalize updated source code
</commit_message>
<xml_diff>
--- a/vcf_stuff/panel_of_normals/pon_eval_mb_100_100.xlsx
+++ b/vcf_stuff/panel_of_normals/pon_eval_mb_100_100.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="42600" yWindow="1340" windowWidth="33460" windowHeight="15720" tabRatio="500"/>
+    <workbookView xWindow="140" yWindow="600" windowWidth="33460" windowHeight="20400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>TP</t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>INDEL</t>
+  </si>
+  <si>
+    <t>mb-ensemble.1sample</t>
+  </si>
+  <si>
+    <t>mb-ensemble.2sample</t>
+  </si>
+  <si>
+    <t>mb-ensemble.3sample</t>
   </si>
 </sst>
 </file>
@@ -492,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,19 +807,19 @@
         <v>0.90593677717810295</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:T23" si="0">C$3-C5</f>
+        <f t="shared" ref="S5:S28" si="0">C$3-C5</f>
         <v>80</v>
       </c>
       <c r="T5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="T5:T28" si="1">D$3-D5</f>
         <v>-10</v>
       </c>
       <c r="V5">
-        <f t="shared" ref="V5:W23" si="1">K$3-K5</f>
+        <f t="shared" ref="V5:V28" si="2">K$3-K5</f>
         <v>33</v>
       </c>
       <c r="W5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="W5:W28" si="3">L$3-L5</f>
         <v>-7</v>
       </c>
     </row>
@@ -871,15 +880,15 @@
         <v>110</v>
       </c>
       <c r="T6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-16</v>
       </c>
       <c r="V6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>317</v>
       </c>
       <c r="W6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-26</v>
       </c>
     </row>
@@ -940,15 +949,15 @@
         <v>63</v>
       </c>
       <c r="T7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9</v>
       </c>
       <c r="V7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="W7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-4</v>
       </c>
     </row>
@@ -1009,15 +1018,15 @@
         <v>93</v>
       </c>
       <c r="T8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-14</v>
       </c>
       <c r="V8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>205</v>
       </c>
       <c r="W8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-20</v>
       </c>
     </row>
@@ -1078,15 +1087,15 @@
         <v>152</v>
       </c>
       <c r="T9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-31</v>
       </c>
       <c r="V9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>870</v>
       </c>
       <c r="W9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-74</v>
       </c>
     </row>
@@ -1147,15 +1156,15 @@
         <v>82</v>
       </c>
       <c r="T10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-13</v>
       </c>
       <c r="V10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
       <c r="W10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-12</v>
       </c>
     </row>
@@ -1216,15 +1225,15 @@
         <v>124</v>
       </c>
       <c r="T11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-25</v>
       </c>
       <c r="V11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>631</v>
       </c>
       <c r="W11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-46</v>
       </c>
     </row>
@@ -1285,15 +1294,15 @@
         <v>65</v>
       </c>
       <c r="T12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-11</v>
       </c>
       <c r="V12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="W12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-9</v>
       </c>
     </row>
@@ -1354,15 +1363,15 @@
         <v>109</v>
       </c>
       <c r="T13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-23</v>
       </c>
       <c r="V13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>480</v>
       </c>
       <c r="W13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-36</v>
       </c>
     </row>
@@ -1423,15 +1432,15 @@
         <v>88</v>
       </c>
       <c r="T14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-11</v>
       </c>
       <c r="V14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="W14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-8</v>
       </c>
     </row>
@@ -1492,15 +1501,15 @@
         <v>68</v>
       </c>
       <c r="T15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9</v>
       </c>
       <c r="V15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="W15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-4</v>
       </c>
     </row>
@@ -1561,15 +1570,15 @@
         <v>69</v>
       </c>
       <c r="T16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9</v>
       </c>
       <c r="V16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="W16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-5</v>
       </c>
     </row>
@@ -1630,15 +1639,15 @@
         <v>55</v>
       </c>
       <c r="T17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-7</v>
       </c>
       <c r="V17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="W17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
     </row>
@@ -1699,15 +1708,15 @@
         <v>55</v>
       </c>
       <c r="T18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-7</v>
       </c>
       <c r="V18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="W18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
     </row>
@@ -1768,15 +1777,15 @@
         <v>91</v>
       </c>
       <c r="T19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-14</v>
       </c>
       <c r="V19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="W19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-14</v>
       </c>
     </row>
@@ -1837,15 +1846,15 @@
         <v>70</v>
       </c>
       <c r="T20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-11</v>
       </c>
       <c r="V20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="W20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-9</v>
       </c>
     </row>
@@ -1906,15 +1915,15 @@
         <v>71</v>
       </c>
       <c r="T21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-11</v>
       </c>
       <c r="V21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="W21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-10</v>
       </c>
     </row>
@@ -1975,15 +1984,15 @@
         <v>57</v>
       </c>
       <c r="T22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-9</v>
       </c>
       <c r="V22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="W22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-6</v>
       </c>
     </row>
@@ -2044,21 +2053,297 @@
         <v>57</v>
       </c>
       <c r="T23">
+        <f t="shared" si="1"/>
+        <v>-9</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="3"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>1185</v>
+      </c>
+      <c r="C25">
+        <v>508</v>
+      </c>
+      <c r="D25">
+        <v>78</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.93824228028503498</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.69994093325457696</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.80175913396481702</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.87842846553002196</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.90735068912710504</v>
+      </c>
+      <c r="J25">
+        <v>318</v>
+      </c>
+      <c r="K25">
+        <v>1364</v>
+      </c>
+      <c r="L25">
+        <v>29</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0.91642651296829902</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0.18906064209274601</v>
+      </c>
+      <c r="O25" s="1">
+        <v>0.31345490389354302</v>
+      </c>
+      <c r="P25" s="1">
+        <v>0.51791530944625397</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>0.90735068912710504</v>
+      </c>
+      <c r="S25">
         <f t="shared" si="0"/>
-        <v>-9</v>
-      </c>
-      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="T25">
         <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>1165</v>
+      </c>
+      <c r="C26">
+        <v>368</v>
+      </c>
+      <c r="D26">
+        <v>98</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.92240696753760798</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.75994781474233497</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.88458618071374295</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.90310077519379806</v>
+      </c>
+      <c r="J26">
+        <v>283</v>
+      </c>
+      <c r="K26">
+        <v>864</v>
+      </c>
+      <c r="L26">
+        <v>64</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0.81556195965417799</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0.24673060156931101</v>
+      </c>
+      <c r="O26" s="1">
+        <v>0.37884872824631799</v>
+      </c>
+      <c r="P26" s="1">
+        <v>0.55818540433925001</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>0.90310077519379806</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="T26">
         <f t="shared" si="1"/>
-        <v>-6</v>
+        <v>-20</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="3"/>
+        <v>-35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>1169</v>
+      </c>
+      <c r="C27">
+        <v>398</v>
+      </c>
+      <c r="D27">
+        <v>94</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.92557403008709405</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.74601148691767705</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.82614840989399296</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0.88306390693458203</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.90381939075305395</v>
+      </c>
+      <c r="J27">
+        <v>301</v>
+      </c>
+      <c r="K27">
+        <v>1012</v>
+      </c>
+      <c r="L27">
+        <v>46</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0.86743515850144004</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0.22924600152322899</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0.36265060240963798</v>
+      </c>
+      <c r="P27" s="1">
+        <v>0.55720103665309095</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>0.90381939075305395</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="1"/>
+        <v>-16</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="2"/>
+        <v>352</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="3"/>
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>1171</v>
+      </c>
+      <c r="C28">
+        <v>415</v>
+      </c>
+      <c r="D28">
+        <v>92</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.92715756136183602</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.73833543505674604</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.82204282204282197</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.88204278397107505</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0.90403767466995999</v>
+      </c>
+      <c r="J28">
+        <v>307</v>
+      </c>
+      <c r="K28">
+        <v>1118</v>
+      </c>
+      <c r="L28">
+        <v>40</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0.88472622478386098</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0.21543859649122801</v>
+      </c>
+      <c r="O28" s="1">
+        <v>0.34650112866817101</v>
+      </c>
+      <c r="P28" s="1">
+        <v>0.54568076786349096</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>0.90403767466995999</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="1"/>
+        <v>-14</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="2"/>
+        <v>246</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="3"/>
+        <v>-11</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G40:G1048576 G2:G23">
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2070,7 +2355,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40:H1048576 H2:H23">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2082,7 +2367,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:I1048576 I2:I23">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2094,7 +2379,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O40:O1048576 O2:O23">
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2106,7 +2391,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P40:P1048576 P2:P23">
-    <cfRule type="colorScale" priority="46">
+    <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2118,7 +2403,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q40:Q1048576 Q2:Q23">
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2130,7 +2415,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E40:E1048576 E2:E23">
-    <cfRule type="colorScale" priority="52">
+    <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2142,7 +2427,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F40:F1048576 F2:F23">
-    <cfRule type="colorScale" priority="55">
+    <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2154,7 +2439,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M40:M1048576 M2:M23">
-    <cfRule type="colorScale" priority="58">
+    <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2166,7 +2451,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40:N1048576 N2:N23">
-    <cfRule type="colorScale" priority="61">
+    <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2178,7 +2463,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U1048576">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2192,7 +2477,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T1048576">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2206,7 +2491,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:T1048576">
-    <cfRule type="dataBar" priority="8">
+    <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2220,7 +2505,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R1048576">
-    <cfRule type="dataBar" priority="14">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2233,8 +2518,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S1048576 T4:T23">
-    <cfRule type="dataBar" priority="12">
+  <conditionalFormatting sqref="S2:S1048576 T4:T28">
+    <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2247,8 +2532,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V1048576 W4:W23">
-    <cfRule type="dataBar" priority="6">
+  <conditionalFormatting sqref="V2:V1048576 W4:W28">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2262,7 +2547,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W1048576">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2276,7 +2561,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:W1048576">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2287,6 +2572,126 @@
           <x14:id>{CFE30A9D-B4AC-3245-BD75-7D899FC8E6BF}</x14:id>
         </ext>
       </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:M1048576">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N1:N1048576">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P1:P1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q1:Q1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2347,7 +2752,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>S2:S1048576 T4:T23</xm:sqref>
+          <xm:sqref>S2:S1048576 T4:T28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F76EE0B7-FCC5-EC41-9FEA-CF0D1B2BAB24}">
@@ -2358,7 +2763,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>V2:V1048576 W4:W23</xm:sqref>
+          <xm:sqref>V2:V1048576 W4:W28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{3E8758EF-F523-C345-A474-DC7B2746380A}">

</xml_diff>